<commit_message>
updating with results for 28 workers, and operation explanation
</commit_message>
<xml_diff>
--- a/Results and Screenshots/Performance Graph.xlsx
+++ b/Results and Screenshots/Performance Graph.xlsx
@@ -26,10 +26,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Workers</t>
+    <t>Num workers</t>
   </si>
   <si>
-    <t>Time taken</t>
+    <t>Time (Seconds)</t>
   </si>
 </sst>
 </file>
@@ -202,7 +202,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time taken</c:v>
+                  <c:v>Time (Seconds)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -233,10 +233,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -251,16 +251,85 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$B$2:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>121.41626000399999</c:v>
                 </c:pt>
@@ -275,6 +344,75 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>33.873234033599999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.331574201599999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.766283035299999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.078912019699999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.9913759232</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.552531003999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.425837039899999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.976191997499999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.0926380157</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.050382137300002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.9155650139</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.1709301472</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.976074934</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.3067250252</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.7976720333</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.913285970700001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17.253885030700001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16.0006451607</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.827867984800001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16.563597917599999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16.855931043599998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17.747982025100001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17.3928120136</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16.7250189781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -301,7 +439,7 @@
         <c:axId val="382410264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5"/>
+          <c:max val="28"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1438,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,6 +1632,190 @@
         <v>33.873234033599999</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>25.331574201599999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>23.766283035299999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>21.078912019699999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>21.9913759232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>19.552531003999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>18.425837039899999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>17.976191997499999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>17.0926380157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>17.050382137300002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>16.9155650139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>18.1709301472</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>16.976074934</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>15.3067250252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>16.7976720333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>15.913285970700001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>17.253885030700001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>16.0006451607</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>17.827867984800001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>16.563597917599999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>16.855931043599998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>17.747982025100001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>17.3928120136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>16.7250189781</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>